<commit_message>
#1 Accept `Pattern[str]` in `iter_named_range_tables` and `iter_list_object_tables`.
</commit_message>
<xml_diff>
--- a/test_data/tables.xlsx
+++ b/test_data/tables.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\aa\aa-py-openpyxl-util\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD888833-C037-44C7-A1B4-B89BC3EF1A73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3706A19F-6C31-4D6B-9194-8F565F3184B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D24BF1F-7E9A-49AF-8AB3-AB526E442EF5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7D24BF1F-7E9A-49AF-8AB3-AB526E442EF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="FooBar2">Sheet2!$F$2:$H$5</definedName>
     <definedName name="SingleCell1">Sheet1!$H$2</definedName>
     <definedName name="SingleRow1">Sheet1!$J$2:$L$2</definedName>
     <definedName name="Table1">Sheet1!$B$2:$C$4</definedName>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>a</t>
   </si>
@@ -65,14 +67,40 @@
   </si>
   <si>
     <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -88,7 +116,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -162,11 +190,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -174,6 +222,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -197,6 +249,18 @@
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4A9B6351-4CFF-4078-B684-DC6E440903F8}" name="c"/>
     <tableColumn id="2" xr3:uid="{AEE2A4D1-1493-43F6-A7F9-F1DF4636B030}" name="d"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{47C98562-3ECD-437D-A70B-0CB118074A02}" name="FooBar1" displayName="FooBar1" ref="B2:D5" totalsRowShown="0">
+  <autoFilter ref="B2:D5" xr:uid="{47C98562-3ECD-437D-A70B-0CB118074A02}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{F6E9333E-92EB-4FD0-9FB8-21A29334027D}" name="i"/>
+    <tableColumn id="2" xr3:uid="{97E8B1C4-A3A7-49B1-865D-0162D2D2BBD6}" name="j"/>
+    <tableColumn id="3" xr3:uid="{7C1E4798-8147-4334-B42F-3390FB210EEB}" name="k"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -491,7 +555,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -501,7 +565,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B63B779C-AFB5-46CD-B12E-99B9B7D71843}">
   <dimension ref="B2:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -561,4 +625,101 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8C0949-587F-49CC-B9FD-3534F122BA41}">
+  <dimension ref="B2:H5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+      <c r="H3" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>8</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>5</v>
+      </c>
+      <c r="H4" s="2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7">
+        <v>6</v>
+      </c>
+      <c r="H5" s="4">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>